<commit_message>
changed Turkana by Elkartasun taldea
</commit_message>
<xml_diff>
--- a/Kalkulu-orri izengabea.xlsx
+++ b/Kalkulu-orri izengabea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\elkartasuntaldea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE8E179-3A79-41E3-B764-0DB466C5865B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406FEE77-AEC2-4989-82C3-41E829176E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7524" yWindow="984" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="164" formatCode="#,##0&quot;€&quot;"/>
   </numFmts>
@@ -188,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -210,6 +211,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -220,7 +224,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -444,25 +448,25 @@
   <dimension ref="A3:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D16"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -483,7 +487,7 @@
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="8">
         <v>235.6</v>
       </c>
       <c r="D7" s="5">
@@ -505,7 +509,9 @@
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="14">
+        <v>139</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
@@ -513,7 +519,9 @@
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
@@ -521,7 +529,9 @@
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
@@ -529,7 +539,9 @@
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4">
+        <v>101.14</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>

</xml_diff>

<commit_message>
funding details in excel updated
</commit_message>
<xml_diff>
--- a/Kalkulu-orri izengabea.xlsx
+++ b/Kalkulu-orri izengabea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\elkartasuntaldea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2947D04D-0AD1-4035-A7B4-26CCADBDB2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A35724-25D0-46CF-A9F5-755F34ED0332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -201,6 +201,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -210,9 +213,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,25 +434,25 @@
   <dimension ref="A3:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -473,95 +473,107 @@
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="6">
         <v>235.6</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="6">
         <v>993</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="6">
         <v>185</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="D8" s="6">
+        <v>321</v>
+      </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="6">
         <v>139</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="D9" s="6">
+        <v>454.1</v>
+      </c>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="6">
         <v>0</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="6">
         <v>0</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="6">
         <v>101.14</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="D12" s="6">
+        <v>340</v>
+      </c>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="C13" s="6">
+        <v>25</v>
+      </c>
+      <c r="D13" s="6">
+        <v>322</v>
+      </c>
+      <c r="E13" s="6">
+        <v>125</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="19" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>

</xml_diff>